<commit_message>
Updated histogram information and truth data to show good patients
</commit_message>
<xml_diff>
--- a/Symmetry Code (Final)/TruthData.xlsx
+++ b/Symmetry Code (Final)/TruthData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shann\Box\GRP_Loew-Doc\NadaKamona\Shannon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smbailes\Documents\GitHub\loewlab\Symmetry Code (Final)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{818E6CD8-DCCD-44CB-8096-220B511ABFC3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,8 +110,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,13 +127,55 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,14 +187,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,23 +516,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052F4A00-00E7-4532-8BEF-FA80F738E666}">
-  <dimension ref="A1:H15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" customWidth="1"/>
-    <col min="7" max="7" width="2.1796875" customWidth="1"/>
-    <col min="8" max="8" width="55.90625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="55.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -499,282 +551,282 @@
       <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>5.3</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <v>1.6</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="5">
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>2</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>2</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>11</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>2.6</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>11</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>1.5</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>9</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>10</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>1.2</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>1.3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>3</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>3</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>1.2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>4</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H10" t="s">
+      <c r="G10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>9</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>7</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>2.4</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>12</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>2</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <v>1.3</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="4">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>5</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>5</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>1</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>1</v>
       </c>
-      <c r="H13" t="s">
+      <c r="G13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>3</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>6</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>1.3</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>0.5</v>
       </c>
-      <c r="H14" t="s">
+      <c r="G14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>10</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>9</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>1.6</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>2.2999999999999998</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated truth table and images
</commit_message>
<xml_diff>
--- a/Symmetry Code (Final)/TruthData.xlsx
+++ b/Symmetry Code (Final)/TruthData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shann\Box\GRP_Loew-Doc\NadaKamona\Shannon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sydney\Documents\GitHub\loewlab\Symmetry Code (Final)\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CF135DB1-A6D6-4DAA-ABDB-3798861CC64A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{818E6CD8-DCCD-44CB-8096-220B511ABFC3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6942" xr2:uid="{818E6CD8-DCCD-44CB-8096-220B511ABFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>IRST001</t>
   </si>
@@ -105,6 +106,18 @@
   </si>
   <si>
     <t>spiculated mass, lower-outer, no distance given</t>
+  </si>
+  <si>
+    <t>IRST015</t>
+  </si>
+  <si>
+    <t>IRST016</t>
+  </si>
+  <si>
+    <t>Upper outer; unknown size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right </t>
   </si>
 </sst>
 </file>
@@ -465,22 +478,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052F4A00-00E7-4532-8BEF-FA80F738E666}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" customWidth="1"/>
-    <col min="7" max="7" width="2.1796875" customWidth="1"/>
-    <col min="8" max="8" width="55.90625" customWidth="1"/>
+    <col min="2" max="2" width="11.47265625" customWidth="1"/>
+    <col min="3" max="3" width="10.62890625" customWidth="1"/>
+    <col min="4" max="4" width="12.26171875" customWidth="1"/>
+    <col min="7" max="7" width="2.15625" customWidth="1"/>
+    <col min="8" max="8" width="55.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -503,7 +516,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -526,7 +539,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -546,7 +559,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -569,7 +582,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -589,7 +602,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -609,7 +622,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -629,7 +642,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -649,7 +662,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -672,7 +685,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -692,7 +705,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -712,7 +725,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -735,7 +748,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -758,7 +771,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -776,6 +789,49 @@
       </c>
       <c r="F15">
         <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F17">
+        <v>2.2000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>